<commit_message>
Switched over the computations to R 03182021
</commit_message>
<xml_diff>
--- a/Execution_Stats.xlsx
+++ b/Execution_Stats.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vdeshpande\Desktop\Del_Project-Takeda\Site_Master_Repo\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C3B82F1E-353A-4BD7-AA92-8F5988886F47}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F3FA5A6F-75EC-4EE1-9D4A-24BCF302C179}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029" calcOnSave="0"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -389,7 +389,7 @@
   <dimension ref="A1:F5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -478,11 +478,11 @@
         <v>6</v>
       </c>
       <c r="E4">
-        <v>4353</v>
+        <v>5124</v>
       </c>
       <c r="F4">
         <f>E4/60</f>
-        <v>72.55</v>
+        <v>85.4</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.35">

</xml_diff>

<commit_message>
Working version for dedup and added recursive processing strategy 24032021
</commit_message>
<xml_diff>
--- a/Execution_Stats.xlsx
+++ b/Execution_Stats.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vdeshpande\Desktop\Del_Project-Takeda\Site_Master_Repo\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F3FA5A6F-75EC-4EE1-9D4A-24BCF302C179}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D50BFA79-69F1-4FB2-ADA1-17B6967E8C7A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="7">
   <si>
     <t>Combination</t>
   </si>
@@ -47,25 +47,13 @@
     <t>Single Country</t>
   </si>
   <si>
-    <t>With_Parallel_Processing</t>
-  </si>
-  <si>
-    <t>N</t>
-  </si>
-  <si>
-    <t>Yes</t>
-  </si>
-  <si>
-    <t>&gt;7200</t>
-  </si>
-  <si>
-    <t>&gt;2 hours</t>
-  </si>
-  <si>
     <t>Time_Required (Mins)</t>
   </si>
   <si>
     <t>Time_Required (Sec)</t>
+  </si>
+  <si>
+    <t>RAM usage crashes code</t>
   </si>
 </sst>
 </file>
@@ -89,7 +77,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -97,15 +85,29 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -386,10 +388,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F5"/>
+  <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -397,112 +399,82 @@
     <col min="1" max="1" width="12.7265625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="18.453125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="14.36328125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="21.90625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="18" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="19.453125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="19.453125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="21.54296875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A1" t="s">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="E1" t="s">
-        <v>10</v>
-      </c>
-      <c r="F1" t="s">
-        <v>9</v>
+      <c r="E1" s="1" t="s">
+        <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A2" t="s">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A2" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B2">
-        <v>300</v>
-      </c>
-      <c r="C2">
-        <v>44850</v>
-      </c>
-      <c r="D2" t="s">
+      <c r="B2" s="1">
+        <v>3500</v>
+      </c>
+      <c r="C2" s="1">
+        <f>B2*(B2-1)/2</f>
+        <v>6123250</v>
+      </c>
+      <c r="D2" s="1">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="E2" s="1">
+        <f>D2*60</f>
+        <v>132</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A3" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3" s="1">
+        <v>5000</v>
+      </c>
+      <c r="C3" s="1">
+        <f>B3*(B3-1)/2</f>
+        <v>12497500</v>
+      </c>
+      <c r="D3" s="1">
+        <f>(C3/C2)*D2</f>
+        <v>4.4901808680031037</v>
+      </c>
+      <c r="E3" s="1">
+        <f>D3*60</f>
+        <v>269.4108520801862</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A4" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4" s="2">
+        <v>20398</v>
+      </c>
+      <c r="C4" s="1">
+        <f>B4*(B4-1)/2</f>
+        <v>208029003</v>
+      </c>
+      <c r="D4" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="E2">
-        <v>210</v>
-      </c>
-      <c r="F2">
-        <f>E2/60</f>
-        <v>3.5</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A3" t="s">
-        <v>3</v>
-      </c>
-      <c r="B3">
-        <v>300</v>
-      </c>
-      <c r="C3">
-        <v>44850</v>
-      </c>
-      <c r="D3" t="s">
-        <v>5</v>
-      </c>
-      <c r="E3">
-        <v>3000</v>
-      </c>
-      <c r="F3">
-        <f>E3/60</f>
-        <v>50</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A4" t="s">
-        <v>3</v>
-      </c>
-      <c r="B4">
-        <v>1371</v>
-      </c>
-      <c r="C4">
-        <v>939135</v>
-      </c>
-      <c r="D4" t="s">
+      <c r="E4" s="1" t="s">
         <v>6</v>
-      </c>
-      <c r="E4">
-        <v>5124</v>
-      </c>
-      <c r="F4">
-        <f>E4/60</f>
-        <v>85.4</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A5" t="s">
-        <v>3</v>
-      </c>
-      <c r="B5">
-        <v>1371</v>
-      </c>
-      <c r="C5">
-        <v>939135</v>
-      </c>
-      <c r="D5" t="s">
-        <v>5</v>
-      </c>
-      <c r="E5" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="F5" s="1" t="s">
-        <v>8</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Attempted source-SQL read. Server has outdated version of Python, so pyodbc didn't work. 04052021
</commit_message>
<xml_diff>
--- a/Execution_Stats.xlsx
+++ b/Execution_Stats.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vdeshpande\Desktop\Del_Project-Takeda\Site_Master_Repo\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D50BFA79-69F1-4FB2-ADA1-17B6967E8C7A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{80311AEB-149C-4E0F-A22B-995FC6CAE2FD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="191029" calcOnSave="0"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="7">
   <si>
     <t>Combination</t>
   </si>
@@ -104,10 +104,15 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="3" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -388,10 +393,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E4"/>
+  <dimension ref="A1:G5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+      <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -399,11 +404,11 @@
     <col min="1" max="1" width="12.7265625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="18.453125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="14.36328125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="19.453125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="21.54296875" customWidth="1"/>
     <col min="5" max="5" width="21.54296875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -420,60 +425,87 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="1">
+      <c r="B2" s="3">
         <v>3500</v>
       </c>
-      <c r="C2" s="1">
+      <c r="C2" s="3">
         <f>B2*(B2-1)/2</f>
         <v>6123250</v>
       </c>
-      <c r="D2" s="1">
+      <c r="D2" s="2">
         <v>2.2000000000000002</v>
       </c>
-      <c r="E2" s="1">
+      <c r="E2" s="2">
         <f>D2*60</f>
         <v>132</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="1">
+      <c r="B3" s="3">
         <v>5000</v>
       </c>
-      <c r="C3" s="1">
+      <c r="C3" s="3">
         <f>B3*(B3-1)/2</f>
         <v>12497500</v>
       </c>
-      <c r="D3" s="1">
+      <c r="D3" s="2">
         <f>(C3/C2)*D2</f>
         <v>4.4901808680031037</v>
       </c>
-      <c r="E3" s="1">
+      <c r="E3" s="2">
         <f>D3*60</f>
         <v>269.4108520801862</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="2">
+      <c r="B4" s="3">
+        <v>14911</v>
+      </c>
+      <c r="C4" s="3">
+        <f>B4*(B4-1)/2</f>
+        <v>111161505</v>
+      </c>
+      <c r="D4" s="2">
+        <f>(C4/C3)*D3</f>
+        <v>39.938808802515005</v>
+      </c>
+      <c r="E4" s="2">
+        <f>D4*60</f>
+        <v>2396.3285281509002</v>
+      </c>
+      <c r="F4" s="1">
+        <v>20.2</v>
+      </c>
+      <c r="G4" s="1">
+        <f>F4*60</f>
+        <v>1212</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A5" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B5" s="3">
         <v>20398</v>
       </c>
-      <c r="C4" s="1">
-        <f>B4*(B4-1)/2</f>
+      <c r="C5" s="3">
+        <f>B5*(B5-1)/2</f>
         <v>208029003</v>
       </c>
-      <c r="D4" s="1" t="s">
+      <c r="D5" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="E4" s="1" t="s">
+      <c r="E5" s="2" t="s">
         <v>6</v>
       </c>
     </row>

</xml_diff>